<commit_message>
Auswertung 6 Bloecke ergaenzt
</commit_message>
<xml_diff>
--- a/Praktikum3/Performance_Uebersicht.xlsx
+++ b/Praktikum3/Performance_Uebersicht.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5 Blöcke" sheetId="1" r:id="rId1"/>
+    <sheet name="6 Blöcke" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Performnace</t>
   </si>
@@ -56,6 +57,18 @@
   </si>
   <si>
     <t>Bergsteigen mit Backtracking</t>
+  </si>
+  <si>
+    <t>6 Blöcke</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2,846,413</t>
+  </si>
+  <si>
+    <t>0.953</t>
   </si>
 </sst>
 </file>
@@ -1456,6 +1469,331 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100"/>
             <a:t>Action: put_on(block5,block3)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1910972" cy="2503506"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="2105025"/>
+          <a:ext cx="1910972" cy="2503506"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>SOLUTION (A):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: start</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block3)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on_table(block3)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on_table(block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on_table(block1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block1,block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block2,block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block4,block6)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2016514" cy="4225772"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Textfeld 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2600325" y="2133600"/>
+          <a:ext cx="2016514" cy="4225772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>SOLUTION (Bergsteigen mit BT):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: start</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on_table(block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block5,block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block3)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on_table(block3)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block4,block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block3,block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block5,block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block6,block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on_table(block1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block1,block4)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block4,block6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: pick_up(block5)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Action: put_on(block2,block5)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1754,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,4 +2179,99 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>13.551</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>179.11600000000001</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>